<commit_message>
Adding iteration 4 close out document updates
</commit_message>
<xml_diff>
--- a/assignment-documents/Iteration4/RedEyesBlackDragons_Actual_Effort.xlsx
+++ b/assignment-documents/Iteration4/RedEyesBlackDragons_Actual_Effort.xlsx
@@ -4658,7 +4658,7 @@
       <c r="H65" s="108"/>
       <c r="I65" s="116">
         <f>SUM(H66:H70)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -4828,12 +4828,24 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="125"/>
-      <c r="N68" s="125"/>
-      <c r="O68" s="125"/>
-      <c r="P68" s="125"/>
-      <c r="Q68" s="125"/>
-      <c r="R68" s="125"/>
+      <c r="M68" s="122">
+        <v>8.0</v>
+      </c>
+      <c r="N68" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="O68" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="P68" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="Q68" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="R68" s="122">
+        <v>0.0</v>
+      </c>
       <c r="S68" s="123"/>
       <c r="T68" s="4"/>
       <c r="U68" s="4"/>
@@ -4868,18 +4880,30 @@
       </c>
       <c r="G69" s="121"/>
       <c r="H69" s="48">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I69" s="121"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="122"/>
-      <c r="N69" s="122"/>
-      <c r="O69" s="122"/>
-      <c r="P69" s="122"/>
-      <c r="Q69" s="122"/>
-      <c r="R69" s="122"/>
+      <c r="M69" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="N69" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="O69" s="122">
+        <v>1.0</v>
+      </c>
+      <c r="P69" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="Q69" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="R69" s="122">
+        <v>0.0</v>
+      </c>
       <c r="S69" s="123"/>
       <c r="T69" s="4"/>
       <c r="U69" s="4"/>

</xml_diff>